<commit_message>
updates and a new file
</commit_message>
<xml_diff>
--- a/SCHEDULER.xlsx
+++ b/SCHEDULER.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="343">
   <si>
     <t>#</t>
   </si>
@@ -1047,6 +1047,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Python Bootcamp (Udemy)</t>
+  </si>
+  <si>
+    <t>EPAT (QuantInsti)</t>
   </si>
 </sst>
 </file>
@@ -1507,22 +1513,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BG222"/>
+  <dimension ref="A1:BG233"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomRight" activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="2" width="38.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3"/>
+    <col min="3" max="3" width="9.140625" style="3"/>
+    <col min="4" max="4" width="0" style="3" hidden="1" customWidth="1"/>
     <col min="5" max="12" width="9.140625" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="9.140625" style="3" collapsed="1"/>
+    <col min="13" max="13" width="0" style="3" hidden="1" customWidth="1"/>
     <col min="14" max="19" width="9.140625" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="20" max="20" width="9.140625" style="3" collapsed="1"/>
     <col min="21" max="16384" width="9.140625" style="3"/>
@@ -1776,7 +1783,7 @@
       <c r="AD3" s="9"/>
       <c r="AE3" s="9"/>
     </row>
-    <row r="4" spans="1:59" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:59" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <v>1</v>
       </c>
@@ -1787,7 +1794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:59" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:59" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -1824,7 +1831,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:59" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:59" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14">
         <v>3</v>
       </c>
@@ -1858,7 +1865,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:59" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:59" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14">
         <v>4</v>
       </c>
@@ -1892,7 +1899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:59" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:59" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>5</v>
       </c>
@@ -1915,7 +1922,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:59" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:59" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14">
         <v>6</v>
       </c>
@@ -1939,12 +1946,12 @@
       <c r="M9" s="14">
         <v>2</v>
       </c>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="18"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
       <c r="T9" s="14">
         <v>3</v>
       </c>
@@ -1952,7 +1959,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:59" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:59" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14">
         <v>7</v>
       </c>
@@ -1976,12 +1983,12 @@
       <c r="M10" s="14">
         <v>2</v>
       </c>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
       <c r="T10" s="14">
         <v>3</v>
       </c>
@@ -1989,7 +1996,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:59" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:59" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>8</v>
       </c>
@@ -2012,7 +2019,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:59" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:59" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>9</v>
       </c>
@@ -2035,7 +2042,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:59" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:59" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>10</v>
       </c>
@@ -2067,6 +2074,7 @@
         <v>8</v>
       </c>
     </row>
+    <row r="14" spans="1:59" collapsed="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>14</v>
@@ -2102,7 +2110,7 @@
       <c r="AD15" s="9"/>
       <c r="AE15" s="9"/>
     </row>
-    <row r="16" spans="1:59" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:59" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
         <v>1</v>
       </c>
@@ -2113,7 +2121,7 @@
         <v>42401</v>
       </c>
     </row>
-    <row r="17" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10">
         <v>2</v>
       </c>
@@ -2121,7 +2129,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>3</v>
       </c>
@@ -2144,7 +2152,7 @@
       <c r="R18" s="18"/>
       <c r="S18" s="18"/>
     </row>
-    <row r="19" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>4</v>
       </c>
@@ -2168,7 +2176,7 @@
       <c r="R19" s="18"/>
       <c r="S19" s="18"/>
     </row>
-    <row r="20" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>5</v>
       </c>
@@ -2195,7 +2203,7 @@
       <c r="R20" s="14"/>
       <c r="S20" s="14"/>
     </row>
-    <row r="21" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>6</v>
       </c>
@@ -2203,7 +2211,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>7</v>
       </c>
@@ -2216,7 +2224,7 @@
       <c r="M22" s="5"/>
       <c r="T22" s="5"/>
     </row>
-    <row r="23" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>8</v>
       </c>
@@ -2231,7 +2239,7 @@
       <c r="V23" s="5"/>
       <c r="W23" s="5"/>
     </row>
-    <row r="24" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>9</v>
       </c>
@@ -2243,7 +2251,7 @@
       </c>
       <c r="T24" s="5"/>
     </row>
-    <row r="25" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>10</v>
       </c>
@@ -2252,7 +2260,7 @@
       </c>
       <c r="V25" s="5"/>
     </row>
-    <row r="26" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>11</v>
       </c>
@@ -2261,7 +2269,7 @@
       </c>
       <c r="W26" s="5"/>
     </row>
-    <row r="27" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>12</v>
       </c>
@@ -2269,6 +2277,7 @@
         <v>26</v>
       </c>
     </row>
+    <row r="28" spans="1:31" collapsed="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:31" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
         <v>27</v>
@@ -2433,7 +2442,7 @@
       <c r="AD38" s="9"/>
       <c r="AE38" s="9"/>
     </row>
-    <row r="39" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A39" s="13">
         <v>1</v>
       </c>
@@ -2723,7 +2732,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="75" spans="1:19" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:19" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A75" s="13">
         <v>2</v>
       </c>
@@ -2844,7 +2853,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="88" spans="1:19" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:19" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A88" s="13">
         <v>3</v>
       </c>
@@ -3173,7 +3182,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="127" spans="1:19" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:19" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A127" s="7">
         <v>4</v>
       </c>
@@ -3670,7 +3679,8 @@
         <v>180</v>
       </c>
     </row>
-    <row r="187" spans="1:31" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2"/>
+    <row r="187" spans="1:31" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2"/>
+    <row r="188" spans="1:31" collapsed="1" x14ac:dyDescent="0.2"/>
     <row r="189" spans="1:31" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A189" s="16" t="s">
         <v>185</v>
@@ -3822,7 +3832,7 @@
       <c r="AD197" s="9"/>
       <c r="AE197" s="9"/>
     </row>
-    <row r="198" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A198" s="12">
         <v>1</v>
       </c>
@@ -3830,7 +3840,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="199" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A199" s="12" t="s">
         <v>209</v>
       </c>
@@ -3839,7 +3849,7 @@
       </c>
       <c r="C199" s="18"/>
     </row>
-    <row r="200" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A200" s="12" t="s">
         <v>210</v>
       </c>
@@ -3848,7 +3858,7 @@
       </c>
       <c r="C200" s="18"/>
     </row>
-    <row r="201" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A201" s="12" t="s">
         <v>211</v>
       </c>
@@ -3856,7 +3866,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="202" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A202" s="12" t="s">
         <v>212</v>
       </c>
@@ -3864,7 +3874,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="203" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A203" s="12" t="s">
         <v>213</v>
       </c>
@@ -3872,7 +3882,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="204" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A204" s="12" t="s">
         <v>205</v>
       </c>
@@ -3880,7 +3890,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="205" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A205" s="12" t="s">
         <v>206</v>
       </c>
@@ -3888,7 +3898,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="206" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A206" s="12" t="s">
         <v>207</v>
       </c>
@@ -3896,7 +3906,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="207" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A207" s="12" t="s">
         <v>208</v>
       </c>
@@ -3904,7 +3914,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="208" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A208" s="12" t="s">
         <v>204</v>
       </c>
@@ -3912,7 +3922,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="209" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A209" s="12" t="s">
         <v>214</v>
       </c>
@@ -3920,7 +3930,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="210" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A210" s="12" t="s">
         <v>215</v>
       </c>
@@ -3928,7 +3938,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="211" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A211" s="12" t="s">
         <v>216</v>
       </c>
@@ -3936,7 +3946,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="212" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A212" s="12">
         <v>2</v>
       </c>
@@ -3944,7 +3954,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="213" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A213" s="12">
         <v>2.1</v>
       </c>
@@ -3953,7 +3963,7 @@
       </c>
       <c r="C213" s="18"/>
     </row>
-    <row r="214" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A214" s="12">
         <v>2.2000000000000002</v>
       </c>
@@ -3962,23 +3972,94 @@
       </c>
       <c r="C214" s="5"/>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A220" s="18"/>
-      <c r="B220" s="3" t="s">
+    <row r="215" spans="1:31" collapsed="1" x14ac:dyDescent="0.2"/>
+    <row r="223" spans="1:31" collapsed="1" x14ac:dyDescent="0.2">
+      <c r="A223" s="16" t="s">
+        <v>341</v>
+      </c>
+      <c r="B223" s="9"/>
+      <c r="C223" s="9"/>
+      <c r="D223" s="9"/>
+      <c r="E223" s="9"/>
+      <c r="F223" s="9"/>
+      <c r="G223" s="9"/>
+      <c r="H223" s="9"/>
+      <c r="I223" s="9"/>
+      <c r="J223" s="9"/>
+      <c r="K223" s="9"/>
+      <c r="L223" s="9"/>
+      <c r="M223" s="9"/>
+      <c r="N223" s="9"/>
+      <c r="O223" s="9"/>
+      <c r="P223" s="9"/>
+      <c r="Q223" s="9"/>
+      <c r="R223" s="9"/>
+      <c r="S223" s="9"/>
+      <c r="T223" s="9"/>
+      <c r="U223" s="9"/>
+      <c r="V223" s="9"/>
+      <c r="W223" s="9"/>
+      <c r="X223" s="9"/>
+      <c r="Y223" s="9"/>
+      <c r="Z223" s="9"/>
+      <c r="AA223" s="9"/>
+      <c r="AB223" s="9"/>
+      <c r="AC223" s="9"/>
+      <c r="AD223" s="9"/>
+      <c r="AE223" s="9"/>
+    </row>
+    <row r="226" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A226" s="18"/>
+      <c r="B226" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A221" s="14"/>
-      <c r="B221" s="3" t="s">
+    <row r="227" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A227" s="14"/>
+      <c r="B227" s="3" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A222" s="5"/>
-      <c r="B222" s="3" t="s">
+    <row r="228" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A228" s="5"/>
+      <c r="B228" s="3" t="s">
         <v>183</v>
       </c>
+    </row>
+    <row r="233" spans="1:31" collapsed="1" x14ac:dyDescent="0.2">
+      <c r="A233" s="16" t="s">
+        <v>342</v>
+      </c>
+      <c r="B233" s="9"/>
+      <c r="C233" s="9"/>
+      <c r="D233" s="9"/>
+      <c r="E233" s="9"/>
+      <c r="F233" s="9"/>
+      <c r="G233" s="9"/>
+      <c r="H233" s="9"/>
+      <c r="I233" s="9"/>
+      <c r="J233" s="9"/>
+      <c r="K233" s="9"/>
+      <c r="L233" s="9"/>
+      <c r="M233" s="9"/>
+      <c r="N233" s="9"/>
+      <c r="O233" s="9"/>
+      <c r="P233" s="9"/>
+      <c r="Q233" s="9"/>
+      <c r="R233" s="9"/>
+      <c r="S233" s="9"/>
+      <c r="T233" s="9"/>
+      <c r="U233" s="9"/>
+      <c r="V233" s="9"/>
+      <c r="W233" s="9"/>
+      <c r="X233" s="9"/>
+      <c r="Y233" s="9"/>
+      <c r="Z233" s="9"/>
+      <c r="AA233" s="9"/>
+      <c r="AB233" s="9"/>
+      <c r="AC233" s="9"/>
+      <c r="AD233" s="9"/>
+      <c r="AE233" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>